<commit_message>
add Gaussian_filter & update all the WorkTools
</commit_message>
<xml_diff>
--- a/003_L946_LA_Force_Pre-Press/configurations_general.xlsx
+++ b/003_L946_LA_Force_Pre-Press/configurations_general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://continental-my.sharepoint.com/personal/uie96795_contiwan_com/Documents/Documents-OneDrive/18_PythonScripts/001_HighSpeed/add_muti-sheet_functuon/003_L946_LA_Force_Pre-Press/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renray/002_PycharmProjects/001_Jupyter_Project/004_Project_Work/007_Tools_Git/WorkTools/003_L946_LA_Force_Pre-Press/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{3AEB96B4-1EFD-4967-AFE5-9135EE13A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5652E0-CEEA-4015-B139-F161EE655716}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6737EBC6-353C-5542-88FF-6BEAD62CA9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="391" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="27700" windowHeight="15720" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="17" r:id="rId1"/>
@@ -229,12 +229,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -541,17 +540,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6856C6C7-06B7-4B79-AF8E-7FB4D3F7D915}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.5" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -559,20 +558,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -584,23 +583,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="88.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="3" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="88.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -635,45 +634,45 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>225615313</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>235538362</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>30</v>
       </c>
@@ -696,7 +695,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -719,7 +718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>28</v>
       </c>
@@ -742,7 +741,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>29</v>
       </c>
@@ -781,19 +780,19 @@
       <selection activeCell="F3" sqref="F3:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="3" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.5" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -828,45 +827,45 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>225615313</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>235538362</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>30</v>
       </c>
@@ -889,7 +888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>31</v>
       </c>
@@ -912,7 +911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>28</v>
       </c>
@@ -935,7 +934,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>29</v>
       </c>

</xml_diff>